<commit_message>
Added 3 combination RAS in vitro findings for DCV after confirmation from Emma
</commit_message>
<xml_diff>
--- a/tabular/contributed/190408 DCV TABLE.xlsx
+++ b/tabular/contributed/190408 DCV TABLE.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3315" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3342" uniqueCount="364">
   <si>
     <t>Weight of evidence</t>
   </si>
@@ -1615,11 +1615,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P385"/>
+  <dimension ref="A1:P388"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A356" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C366" sqref="C366"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A379" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I390" sqref="I390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15959,6 +15959,102 @@
         <v>28789880</v>
       </c>
     </row>
+    <row r="386" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A386" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B386" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C386" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="D386" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E386" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F386" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G386" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H386" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I386" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="O386" s="2">
+        <v>29425396</v>
+      </c>
+    </row>
+    <row r="387" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A387" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B387" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C387" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D387" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E387" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F387" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G387" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H387" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I387" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="O387" s="2">
+        <v>29425396</v>
+      </c>
+    </row>
+    <row r="388" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A388" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B388" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C388" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D388" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E388" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F388" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G388" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H388" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I388" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="O388" s="2">
+        <v>29425396</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
removed DCV in vitro findings superceded by those with more accurate replicon system subtype recorded.
</commit_message>
<xml_diff>
--- a/tabular/contributed/190408 DCV TABLE.xlsx
+++ b/tabular/contributed/190408 DCV TABLE.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3342" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3327" uniqueCount="364">
   <si>
     <t>Weight of evidence</t>
   </si>
@@ -1615,11 +1615,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P388"/>
+  <dimension ref="A1:P385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A379" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I390" sqref="I390"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A373" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A297" sqref="A297:XFD299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12356,118 +12356,150 @@
       <c r="P296" s="11"/>
     </row>
     <row r="297" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A297" s="9">
+      <c r="A297" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B297" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C297" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="D297" s="11"/>
-      <c r="E297" s="11"/>
+        <v>165</v>
+      </c>
+      <c r="D297" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E297" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="F297" s="11"/>
       <c r="G297" s="15" t="s">
         <v>115</v>
       </c>
       <c r="H297" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I297" s="25" t="s">
-        <v>348</v>
-      </c>
-      <c r="J297" s="11"/>
-      <c r="K297" s="11"/>
-      <c r="L297" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="I297" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J297" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="K297" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="L297" s="11" t="s">
+        <v>138</v>
+      </c>
       <c r="M297" s="11"/>
       <c r="N297" s="11"/>
       <c r="O297" s="11">
-        <v>29425396</v>
+        <v>29599611</v>
       </c>
       <c r="P297" s="11"/>
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A298" s="9">
+      <c r="A298" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B298" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C298" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="D298" s="11"/>
-      <c r="E298" s="11"/>
+        <v>166</v>
+      </c>
+      <c r="D298" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E298" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="F298" s="11"/>
       <c r="G298" s="15" t="s">
         <v>115</v>
       </c>
       <c r="H298" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I298" s="25" t="s">
-        <v>348</v>
-      </c>
-      <c r="J298" s="11"/>
-      <c r="K298" s="11"/>
-      <c r="L298" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="I298" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J298" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="K298" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="L298" s="11" t="s">
+        <v>138</v>
+      </c>
       <c r="M298" s="11"/>
       <c r="N298" s="11"/>
       <c r="O298" s="11">
-        <v>29425396</v>
+        <v>29599611</v>
       </c>
       <c r="P298" s="11"/>
     </row>
     <row r="299" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A299" s="9">
+      <c r="A299" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B299" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C299" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D299" s="11"/>
-      <c r="E299" s="11"/>
+        <v>168</v>
+      </c>
+      <c r="D299" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E299" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="F299" s="11"/>
       <c r="G299" s="15" t="s">
         <v>115</v>
       </c>
       <c r="H299" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I299" s="25" t="s">
-        <v>348</v>
-      </c>
-      <c r="J299" s="11"/>
-      <c r="K299" s="11"/>
-      <c r="L299" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="I299" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J299" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="K299" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="L299" s="11" t="s">
+        <v>138</v>
+      </c>
       <c r="M299" s="11"/>
       <c r="N299" s="11"/>
       <c r="O299" s="11">
-        <v>29425396</v>
+        <v>29599611</v>
       </c>
       <c r="P299" s="11"/>
     </row>
     <row r="300" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A300" s="9" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="B300" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C300" s="11" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="D300" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E300" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F300" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="F300" s="11" t="s">
+        <v>140</v>
+      </c>
       <c r="G300" s="15" t="s">
         <v>115</v>
       </c>
@@ -12478,30 +12510,30 @@
         <v>2</v>
       </c>
       <c r="J300" s="11" t="s">
-        <v>137</v>
+        <v>344</v>
       </c>
       <c r="K300" s="11" t="s">
-        <v>90</v>
+        <v>360</v>
       </c>
       <c r="L300" s="11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="M300" s="11"/>
       <c r="N300" s="11"/>
       <c r="O300" s="11">
-        <v>29599611</v>
+        <v>30125371</v>
       </c>
       <c r="P300" s="11"/>
     </row>
     <row r="301" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A301" s="9" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="B301" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C301" s="11" t="s">
-        <v>166</v>
+        <v>276</v>
       </c>
       <c r="D301" s="11" t="s">
         <v>22</v>
@@ -12520,148 +12552,150 @@
         <v>2</v>
       </c>
       <c r="J301" s="11" t="s">
-        <v>137</v>
+        <v>344</v>
       </c>
       <c r="K301" s="11" t="s">
-        <v>90</v>
+        <v>360</v>
       </c>
       <c r="L301" s="11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="M301" s="11"/>
       <c r="N301" s="11"/>
       <c r="O301" s="11">
-        <v>29599611</v>
+        <v>30125371</v>
       </c>
       <c r="P301" s="11"/>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A302" s="9" t="s">
+    <row r="302" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A302" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B302" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C302" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D302" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E302" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F302" s="11"/>
+      <c r="C302" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="D302" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E302" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F302" s="23" t="s">
+        <v>131</v>
+      </c>
       <c r="G302" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H302" s="11" t="s">
+      <c r="H302" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I302" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J302" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="K302" s="11" t="s">
+      <c r="J302" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="K302" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="L302" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="M302" s="11"/>
-      <c r="N302" s="11"/>
-      <c r="O302" s="11">
-        <v>29599611</v>
-      </c>
-      <c r="P302" s="11"/>
-    </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A303" s="9" t="s">
-        <v>139</v>
+      <c r="L302" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="M302" s="23"/>
+      <c r="N302" s="23"/>
+      <c r="O302" s="23">
+        <v>28078469</v>
+      </c>
+      <c r="P302" s="23"/>
+    </row>
+    <row r="303" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A303" s="33" t="s">
+        <v>3</v>
       </c>
       <c r="B303" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C303" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="D303" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E303" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F303" s="11" t="s">
-        <v>140</v>
+      <c r="C303" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="D303" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E303" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F303" s="23" t="s">
+        <v>131</v>
       </c>
       <c r="G303" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H303" s="11" t="s">
+      <c r="H303" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I303" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J303" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="K303" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="L303" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="M303" s="11"/>
-      <c r="N303" s="11"/>
-      <c r="O303" s="11">
-        <v>30125371</v>
-      </c>
-      <c r="P303" s="11"/>
-    </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A304" s="9" t="s">
-        <v>139</v>
+      <c r="J303" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="K303" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="L303" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="M303" s="23"/>
+      <c r="N303" s="23"/>
+      <c r="O303" s="23">
+        <v>28078469</v>
+      </c>
+      <c r="P303" s="23"/>
+    </row>
+    <row r="304" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="33" t="s">
+        <v>3</v>
       </c>
       <c r="B304" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C304" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="D304" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E304" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F304" s="11"/>
+      <c r="C304" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="D304" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E304" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F304" s="23"/>
       <c r="G304" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H304" s="11" t="s">
+      <c r="H304" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I304" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J304" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="K304" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="L304" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="M304" s="11"/>
-      <c r="N304" s="11"/>
-      <c r="O304" s="11">
-        <v>30125371</v>
-      </c>
-      <c r="P304" s="11"/>
+      <c r="J304" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="K304" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="L304" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="M304" s="23"/>
+      <c r="N304" s="23"/>
+      <c r="O304" s="23">
+        <v>28078469</v>
+      </c>
+      <c r="P304" s="23"/>
     </row>
     <row r="305" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A305" s="33" t="s">
@@ -12671,17 +12705,15 @@
         <v>21</v>
       </c>
       <c r="C305" s="23" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D305" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E305" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F305" s="23" t="s">
-        <v>131</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F305" s="23"/>
       <c r="G305" s="15" t="s">
         <v>115</v>
       </c>
@@ -12715,17 +12747,15 @@
         <v>21</v>
       </c>
       <c r="C306" s="23" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D306" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E306" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F306" s="23" t="s">
-        <v>131</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F306" s="23"/>
       <c r="G306" s="15" t="s">
         <v>115</v>
       </c>
@@ -12759,15 +12789,17 @@
         <v>21</v>
       </c>
       <c r="C307" s="23" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D307" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E307" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F307" s="23"/>
+        <v>22</v>
+      </c>
+      <c r="F307" s="23" t="s">
+        <v>145</v>
+      </c>
       <c r="G307" s="15" t="s">
         <v>115</v>
       </c>
@@ -12793,23 +12825,23 @@
       </c>
       <c r="P307" s="23"/>
     </row>
-    <row r="308" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A308" s="33" t="s">
+    <row r="308" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A308" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B308" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C308" s="23" t="s">
-        <v>280</v>
-      </c>
-      <c r="D308" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E308" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F308" s="23"/>
+      <c r="B308" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C308" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="D308" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E308" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F308" s="11"/>
       <c r="G308" s="15" t="s">
         <v>115</v>
       </c>
@@ -12822,36 +12854,36 @@
       <c r="J308" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="K308" s="23" t="s">
+      <c r="K308" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L308" s="23" t="s">
+      <c r="L308" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="M308" s="23"/>
-      <c r="N308" s="23"/>
-      <c r="O308" s="23">
+      <c r="M308" s="11"/>
+      <c r="N308" s="11"/>
+      <c r="O308" s="11">
         <v>28078469</v>
       </c>
-      <c r="P308" s="23"/>
-    </row>
-    <row r="309" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A309" s="33" t="s">
+      <c r="P308" s="11"/>
+    </row>
+    <row r="309" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A309" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B309" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C309" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="D309" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E309" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F309" s="23"/>
+      <c r="B309" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C309" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="D309" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E309" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F309" s="11"/>
       <c r="G309" s="15" t="s">
         <v>115</v>
       </c>
@@ -12864,37 +12896,37 @@
       <c r="J309" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="K309" s="23" t="s">
+      <c r="K309" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L309" s="23" t="s">
+      <c r="L309" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="M309" s="23"/>
-      <c r="N309" s="23"/>
-      <c r="O309" s="23">
+      <c r="M309" s="11"/>
+      <c r="N309" s="11"/>
+      <c r="O309" s="11">
         <v>28078469</v>
       </c>
-      <c r="P309" s="23"/>
-    </row>
-    <row r="310" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A310" s="33" t="s">
+      <c r="P309" s="11"/>
+    </row>
+    <row r="310" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A310" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B310" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C310" s="23" t="s">
-        <v>282</v>
-      </c>
-      <c r="D310" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E310" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F310" s="23" t="s">
-        <v>145</v>
+      <c r="B310" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C310" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="D310" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E310" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F310" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="G310" s="15" t="s">
         <v>115</v>
@@ -12914,12 +12946,12 @@
       <c r="L310" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="M310" s="23"/>
-      <c r="N310" s="23"/>
-      <c r="O310" s="23">
+      <c r="M310" s="11"/>
+      <c r="N310" s="11"/>
+      <c r="O310" s="11">
         <v>28078469</v>
       </c>
-      <c r="P310" s="23"/>
+      <c r="P310" s="11"/>
     </row>
     <row r="311" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A311" s="9" t="s">
@@ -12929,7 +12961,7 @@
         <v>21</v>
       </c>
       <c r="C311" s="11" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D311" s="11" t="s">
         <v>22</v>
@@ -12971,15 +13003,17 @@
         <v>21</v>
       </c>
       <c r="C312" s="11" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D312" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E312" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F312" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="F312" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="G312" s="15" t="s">
         <v>115</v>
       </c>
@@ -13013,17 +13047,15 @@
         <v>21</v>
       </c>
       <c r="C313" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D313" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E313" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F313" s="11" t="s">
-        <v>150</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F313" s="11"/>
       <c r="G313" s="15" t="s">
         <v>115</v>
       </c>
@@ -13036,10 +13068,10 @@
       <c r="J313" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="K313" s="23" t="s">
+      <c r="K313" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L313" s="23" t="s">
+      <c r="L313" s="11" t="s">
         <v>149</v>
       </c>
       <c r="M313" s="11"/>
@@ -13057,15 +13089,17 @@
         <v>21</v>
       </c>
       <c r="C314" s="11" t="s">
-        <v>286</v>
+        <v>175</v>
       </c>
       <c r="D314" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E314" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F314" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="F314" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="G314" s="15" t="s">
         <v>115</v>
       </c>
@@ -13099,7 +13133,7 @@
         <v>21</v>
       </c>
       <c r="C315" s="11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D315" s="11" t="s">
         <v>23</v>
@@ -13107,9 +13141,7 @@
       <c r="E315" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F315" s="11" t="s">
-        <v>132</v>
-      </c>
+      <c r="F315" s="11"/>
       <c r="G315" s="15" t="s">
         <v>115</v>
       </c>
@@ -13143,7 +13175,7 @@
         <v>21</v>
       </c>
       <c r="C316" s="11" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D316" s="11" t="s">
         <v>22</v>
@@ -13185,7 +13217,7 @@
         <v>21</v>
       </c>
       <c r="C317" s="11" t="s">
-        <v>175</v>
+        <v>290</v>
       </c>
       <c r="D317" s="11" t="s">
         <v>23</v>
@@ -13194,7 +13226,7 @@
         <v>22</v>
       </c>
       <c r="F317" s="11" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="G317" s="15" t="s">
         <v>115</v>
@@ -13229,13 +13261,13 @@
         <v>21</v>
       </c>
       <c r="C318" s="11" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D318" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E318" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F318" s="11"/>
       <c r="G318" s="15" t="s">
@@ -13271,15 +13303,17 @@
         <v>21</v>
       </c>
       <c r="C319" s="11" t="s">
-        <v>289</v>
+        <v>174</v>
       </c>
       <c r="D319" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E319" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F319" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="F319" s="11" t="s">
+        <v>143</v>
+      </c>
       <c r="G319" s="15" t="s">
         <v>115</v>
       </c>
@@ -13313,17 +13347,15 @@
         <v>21</v>
       </c>
       <c r="C320" s="11" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D320" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E320" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F320" s="11" t="s">
-        <v>142</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F320" s="11"/>
       <c r="G320" s="15" t="s">
         <v>115</v>
       </c>
@@ -13357,15 +13389,17 @@
         <v>21</v>
       </c>
       <c r="C321" s="11" t="s">
-        <v>291</v>
+        <v>177</v>
       </c>
       <c r="D321" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E321" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F321" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="F321" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="G321" s="15" t="s">
         <v>115</v>
       </c>
@@ -13399,17 +13433,15 @@
         <v>21</v>
       </c>
       <c r="C322" s="11" t="s">
-        <v>174</v>
+        <v>293</v>
       </c>
       <c r="D322" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E322" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F322" s="11" t="s">
-        <v>143</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F322" s="11"/>
       <c r="G322" s="15" t="s">
         <v>115</v>
       </c>
@@ -13443,15 +13475,17 @@
         <v>21</v>
       </c>
       <c r="C323" s="11" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="D323" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E323" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F323" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="F323" s="11" t="s">
+        <v>145</v>
+      </c>
       <c r="G323" s="15" t="s">
         <v>115</v>
       </c>
@@ -13485,17 +13519,15 @@
         <v>21</v>
       </c>
       <c r="C324" s="11" t="s">
-        <v>177</v>
+        <v>294</v>
       </c>
       <c r="D324" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E324" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F324" s="11" t="s">
-        <v>144</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E324" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F324" s="11"/>
       <c r="G324" s="15" t="s">
         <v>115</v>
       </c>
@@ -13529,15 +13561,17 @@
         <v>21</v>
       </c>
       <c r="C325" s="11" t="s">
-        <v>293</v>
+        <v>175</v>
       </c>
       <c r="D325" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E325" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F325" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="F325" s="23" t="s">
+        <v>146</v>
+      </c>
       <c r="G325" s="15" t="s">
         <v>115</v>
       </c>
@@ -13571,17 +13605,15 @@
         <v>21</v>
       </c>
       <c r="C326" s="11" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="D326" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E326" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F326" s="11" t="s">
-        <v>145</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E326" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F326" s="11"/>
       <c r="G326" s="15" t="s">
         <v>115</v>
       </c>
@@ -13615,15 +13647,17 @@
         <v>21</v>
       </c>
       <c r="C327" s="11" t="s">
-        <v>294</v>
+        <v>232</v>
       </c>
       <c r="D327" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E327" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F327" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="E327" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F327" s="11" t="s">
+        <v>147</v>
+      </c>
       <c r="G327" s="15" t="s">
         <v>115</v>
       </c>
@@ -13657,17 +13691,15 @@
         <v>21</v>
       </c>
       <c r="C328" s="11" t="s">
-        <v>175</v>
+        <v>295</v>
       </c>
       <c r="D328" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E328" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F328" s="23" t="s">
-        <v>146</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E328" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F328" s="11"/>
       <c r="G328" s="15" t="s">
         <v>115</v>
       </c>
@@ -13701,15 +13733,17 @@
         <v>21</v>
       </c>
       <c r="C329" s="11" t="s">
-        <v>280</v>
+        <v>175</v>
       </c>
       <c r="D329" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E329" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F329" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="E329" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F329" s="23" t="s">
+        <v>120</v>
+      </c>
       <c r="G329" s="15" t="s">
         <v>115</v>
       </c>
@@ -13743,7 +13777,7 @@
         <v>21</v>
       </c>
       <c r="C330" s="11" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D330" s="11" t="s">
         <v>23</v>
@@ -13752,7 +13786,7 @@
         <v>22</v>
       </c>
       <c r="F330" s="11" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="G330" s="15" t="s">
         <v>115</v>
@@ -13787,7 +13821,7 @@
         <v>21</v>
       </c>
       <c r="C331" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D331" s="11" t="s">
         <v>22</v>
@@ -13829,7 +13863,7 @@
         <v>21</v>
       </c>
       <c r="C332" s="11" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="D332" s="11" t="s">
         <v>23</v>
@@ -13837,8 +13871,8 @@
       <c r="E332" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F332" s="23" t="s">
-        <v>120</v>
+      <c r="F332" s="11" t="s">
+        <v>132</v>
       </c>
       <c r="G332" s="15" t="s">
         <v>115</v>
@@ -13873,17 +13907,15 @@
         <v>21</v>
       </c>
       <c r="C333" s="11" t="s">
-        <v>220</v>
+        <v>297</v>
       </c>
       <c r="D333" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E333" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F333" s="11" t="s">
-        <v>132</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E333" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F333" s="11"/>
       <c r="G333" s="15" t="s">
         <v>115</v>
       </c>
@@ -13917,15 +13949,17 @@
         <v>21</v>
       </c>
       <c r="C334" s="11" t="s">
-        <v>296</v>
+        <v>167</v>
       </c>
       <c r="D334" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E334" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F334" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="E334" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F334" s="11" t="s">
+        <v>148</v>
+      </c>
       <c r="G334" s="15" t="s">
         <v>115</v>
       </c>
@@ -13959,17 +13993,15 @@
         <v>21</v>
       </c>
       <c r="C335" s="11" t="s">
-        <v>190</v>
+        <v>298</v>
       </c>
       <c r="D335" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E335" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F335" s="11" t="s">
-        <v>132</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E335" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F335" s="11"/>
       <c r="G335" s="15" t="s">
         <v>115</v>
       </c>
@@ -14003,7 +14035,7 @@
         <v>21</v>
       </c>
       <c r="C336" s="11" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D336" s="11" t="s">
         <v>22</v>
@@ -14045,7 +14077,7 @@
         <v>21</v>
       </c>
       <c r="C337" s="11" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="D337" s="11" t="s">
         <v>23</v>
@@ -14054,7 +14086,7 @@
         <v>22</v>
       </c>
       <c r="F337" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G337" s="15" t="s">
         <v>115</v>
@@ -14089,7 +14121,7 @@
         <v>21</v>
       </c>
       <c r="C338" s="11" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="D338" s="11" t="s">
         <v>22</v>
@@ -14131,15 +14163,17 @@
         <v>21</v>
       </c>
       <c r="C339" s="11" t="s">
-        <v>299</v>
+        <v>175</v>
       </c>
       <c r="D339" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E339" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F339" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="E339" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F339" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="G339" s="15" t="s">
         <v>115</v>
       </c>
@@ -14173,17 +14207,15 @@
         <v>21</v>
       </c>
       <c r="C340" s="11" t="s">
-        <v>185</v>
+        <v>300</v>
       </c>
       <c r="D340" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E340" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F340" s="11" t="s">
-        <v>145</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E340" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F340" s="11"/>
       <c r="G340" s="15" t="s">
         <v>115</v>
       </c>
@@ -14217,13 +14249,13 @@
         <v>21</v>
       </c>
       <c r="C341" s="11" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="D341" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E341" s="23" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="E341" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="F341" s="11"/>
       <c r="G341" s="15" t="s">
@@ -14259,7 +14291,7 @@
         <v>21</v>
       </c>
       <c r="C342" s="11" t="s">
-        <v>175</v>
+        <v>302</v>
       </c>
       <c r="D342" s="11" t="s">
         <v>23</v>
@@ -14267,9 +14299,7 @@
       <c r="E342" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F342" s="11" t="s">
-        <v>132</v>
-      </c>
+      <c r="F342" s="11"/>
       <c r="G342" s="15" t="s">
         <v>115</v>
       </c>
@@ -14296,22 +14326,24 @@
       <c r="P342" s="11"/>
     </row>
     <row r="343" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A343" s="9" t="s">
+      <c r="A343" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B343" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C343" s="11" t="s">
-        <v>300</v>
+      <c r="C343" s="23" t="s">
+        <v>239</v>
       </c>
       <c r="D343" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E343" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F343" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="E343" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F343" s="23" t="s">
+        <v>24</v>
+      </c>
       <c r="G343" s="15" t="s">
         <v>115</v>
       </c>
@@ -14321,31 +14353,31 @@
       <c r="I343" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J343" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="K343" s="11" t="s">
+      <c r="J343" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K343" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L343" s="11" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="M343" s="11"/>
       <c r="N343" s="11"/>
       <c r="O343" s="11">
-        <v>28078469</v>
+        <v>24444658</v>
       </c>
       <c r="P343" s="11"/>
     </row>
     <row r="344" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A344" s="9" t="s">
+      <c r="A344" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B344" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C344" s="11" t="s">
-        <v>301</v>
+      <c r="C344" s="23" t="s">
+        <v>176</v>
       </c>
       <c r="D344" s="11" t="s">
         <v>23</v>
@@ -14353,7 +14385,9 @@
       <c r="E344" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F344" s="11"/>
+      <c r="F344" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="G344" s="15" t="s">
         <v>115</v>
       </c>
@@ -14363,31 +14397,31 @@
       <c r="I344" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J344" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="K344" s="11" t="s">
+      <c r="J344" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K344" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L344" s="11" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="M344" s="11"/>
       <c r="N344" s="11"/>
       <c r="O344" s="11">
-        <v>28078469</v>
+        <v>24444658</v>
       </c>
       <c r="P344" s="11"/>
     </row>
     <row r="345" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A345" s="9" t="s">
+      <c r="A345" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B345" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C345" s="11" t="s">
-        <v>302</v>
+      <c r="C345" s="23" t="s">
+        <v>241</v>
       </c>
       <c r="D345" s="11" t="s">
         <v>23</v>
@@ -14395,7 +14429,9 @@
       <c r="E345" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F345" s="11"/>
+      <c r="F345" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="G345" s="15" t="s">
         <v>115</v>
       </c>
@@ -14405,19 +14441,19 @@
       <c r="I345" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J345" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="K345" s="11" t="s">
+      <c r="J345" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K345" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L345" s="11" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="M345" s="11"/>
       <c r="N345" s="11"/>
       <c r="O345" s="11">
-        <v>28078469</v>
+        <v>24444658</v>
       </c>
       <c r="P345" s="11"/>
     </row>
@@ -14429,7 +14465,7 @@
         <v>21</v>
       </c>
       <c r="C346" s="23" t="s">
-        <v>239</v>
+        <v>166</v>
       </c>
       <c r="D346" s="11" t="s">
         <v>23</v>
@@ -14438,7 +14474,7 @@
         <v>22</v>
       </c>
       <c r="F346" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G346" s="15" t="s">
         <v>115</v>
@@ -14473,7 +14509,7 @@
         <v>21</v>
       </c>
       <c r="C347" s="23" t="s">
-        <v>176</v>
+        <v>303</v>
       </c>
       <c r="D347" s="11" t="s">
         <v>23</v>
@@ -14481,9 +14517,7 @@
       <c r="E347" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F347" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="F347" s="11"/>
       <c r="G347" s="15" t="s">
         <v>115</v>
       </c>
@@ -14517,7 +14551,7 @@
         <v>21</v>
       </c>
       <c r="C348" s="23" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="D348" s="11" t="s">
         <v>23</v>
@@ -14525,9 +14559,7 @@
       <c r="E348" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F348" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="F348" s="11"/>
       <c r="G348" s="15" t="s">
         <v>115</v>
       </c>
@@ -14541,7 +14573,7 @@
         <v>91</v>
       </c>
       <c r="K348" s="23" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="L348" s="11" t="s">
         <v>153</v>
@@ -14555,13 +14587,13 @@
     </row>
     <row r="349" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A349" s="33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B349" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C349" s="23" t="s">
-        <v>166</v>
+        <v>303</v>
       </c>
       <c r="D349" s="11" t="s">
         <v>23</v>
@@ -14569,9 +14601,7 @@
       <c r="E349" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F349" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="F349" s="11"/>
       <c r="G349" s="15" t="s">
         <v>115</v>
       </c>
@@ -14585,7 +14615,7 @@
         <v>91</v>
       </c>
       <c r="K349" s="23" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="L349" s="11" t="s">
         <v>153</v>
@@ -14599,13 +14629,13 @@
     </row>
     <row r="350" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A350" s="33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B350" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C350" s="23" t="s">
-        <v>303</v>
+        <v>204</v>
       </c>
       <c r="D350" s="11" t="s">
         <v>23</v>
@@ -14627,7 +14657,7 @@
         <v>91</v>
       </c>
       <c r="K350" s="23" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="L350" s="11" t="s">
         <v>153</v>
@@ -14641,19 +14671,19 @@
     </row>
     <row r="351" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A351" s="33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B351" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C351" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="D351" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E351" s="11" t="s">
-        <v>22</v>
+        <v>304</v>
+      </c>
+      <c r="D351" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E351" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="F351" s="11"/>
       <c r="G351" s="15" t="s">
@@ -14669,7 +14699,7 @@
         <v>91</v>
       </c>
       <c r="K351" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L351" s="11" t="s">
         <v>153</v>
@@ -14683,19 +14713,19 @@
     </row>
     <row r="352" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A352" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B352" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C352" s="23" t="s">
-        <v>303</v>
-      </c>
-      <c r="D352" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E352" s="11" t="s">
-        <v>22</v>
+        <v>304</v>
+      </c>
+      <c r="D352" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E352" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="F352" s="11"/>
       <c r="G352" s="15" t="s">
@@ -14711,7 +14741,7 @@
         <v>91</v>
       </c>
       <c r="K352" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L352" s="11" t="s">
         <v>153</v>
@@ -14731,7 +14761,7 @@
         <v>21</v>
       </c>
       <c r="C353" s="23" t="s">
-        <v>204</v>
+        <v>305</v>
       </c>
       <c r="D353" s="11" t="s">
         <v>23</v>
@@ -14753,7 +14783,7 @@
         <v>91</v>
       </c>
       <c r="K353" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L353" s="11" t="s">
         <v>153</v>
@@ -14767,19 +14797,19 @@
     </row>
     <row r="354" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A354" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B354" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C354" s="23" t="s">
-        <v>304</v>
-      </c>
-      <c r="D354" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E354" s="23" t="s">
-        <v>23</v>
+        <v>305</v>
+      </c>
+      <c r="D354" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E354" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="F354" s="11"/>
       <c r="G354" s="15" t="s">
@@ -14809,19 +14839,19 @@
     </row>
     <row r="355" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A355" s="33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B355" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C355" s="23" t="s">
-        <v>304</v>
-      </c>
-      <c r="D355" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E355" s="23" t="s">
-        <v>23</v>
+        <v>163</v>
+      </c>
+      <c r="D355" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E355" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="F355" s="11"/>
       <c r="G355" s="15" t="s">
@@ -14851,13 +14881,13 @@
     </row>
     <row r="356" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A356" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B356" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C356" s="23" t="s">
-        <v>305</v>
+        <v>163</v>
       </c>
       <c r="D356" s="11" t="s">
         <v>23</v>
@@ -14893,13 +14923,13 @@
     </row>
     <row r="357" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A357" s="33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B357" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C357" s="23" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D357" s="11" t="s">
         <v>23</v>
@@ -14935,13 +14965,13 @@
     </row>
     <row r="358" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A358" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B358" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C358" s="23" t="s">
-        <v>163</v>
+        <v>306</v>
       </c>
       <c r="D358" s="11" t="s">
         <v>23</v>
@@ -14977,13 +15007,13 @@
     </row>
     <row r="359" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A359" s="33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B359" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C359" s="23" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="D359" s="11" t="s">
         <v>23</v>
@@ -15019,13 +15049,13 @@
     </row>
     <row r="360" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A360" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B360" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C360" s="23" t="s">
-        <v>306</v>
+        <v>194</v>
       </c>
       <c r="D360" s="11" t="s">
         <v>23</v>
@@ -15061,13 +15091,13 @@
     </row>
     <row r="361" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A361" s="33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B361" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C361" s="23" t="s">
-        <v>306</v>
+        <v>363</v>
       </c>
       <c r="D361" s="11" t="s">
         <v>23</v>
@@ -15103,13 +15133,13 @@
     </row>
     <row r="362" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A362" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B362" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C362" s="23" t="s">
-        <v>194</v>
+        <v>363</v>
       </c>
       <c r="D362" s="11" t="s">
         <v>23</v>
@@ -15145,13 +15175,13 @@
     </row>
     <row r="363" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A363" s="33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B363" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C363" s="23" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="D363" s="11" t="s">
         <v>23</v>
@@ -15187,13 +15217,13 @@
     </row>
     <row r="364" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A364" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B364" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C364" s="23" t="s">
-        <v>363</v>
+        <v>169</v>
       </c>
       <c r="D364" s="11" t="s">
         <v>23</v>
@@ -15227,131 +15257,116 @@
       </c>
       <c r="P364" s="11"/>
     </row>
-    <row r="365" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A365" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B365" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C365" s="23" t="s">
-        <v>363</v>
-      </c>
-      <c r="D365" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E365" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F365" s="11"/>
-      <c r="G365" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="H365" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="I365" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J365" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="K365" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="L365" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="M365" s="11"/>
-      <c r="N365" s="11"/>
-      <c r="O365" s="11">
-        <v>24444658</v>
-      </c>
-      <c r="P365" s="11"/>
-    </row>
-    <row r="366" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A366" s="33" t="s">
+    <row r="365" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B365" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C365" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D365" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E365" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G365" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H365" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I365" s="25"/>
+      <c r="J365" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="K365" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="O365" s="2">
+        <v>26822022</v>
+      </c>
+    </row>
+    <row r="366" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A366" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B366" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C366" s="23" t="s">
+      <c r="B366" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C366" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="D366" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E366" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F366" s="11"/>
-      <c r="G366" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="H366" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="I366" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J366" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="K366" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="L366" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="M366" s="11"/>
-      <c r="N366" s="11"/>
-      <c r="O366" s="11">
-        <v>24444658</v>
-      </c>
-      <c r="P366" s="11"/>
-    </row>
-    <row r="367" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A367" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B367" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C367" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D367" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E367" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F367" s="11"/>
-      <c r="G367" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="H367" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="I367" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J367" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="K367" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="L367" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="M367" s="11"/>
-      <c r="N367" s="11"/>
-      <c r="O367" s="11">
-        <v>24444658</v>
-      </c>
-      <c r="P367" s="11"/>
+      <c r="D366" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E366" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F366" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="G366" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H366" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I366" s="25"/>
+      <c r="J366" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="K366" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="M366" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="O366" s="2">
+        <v>27025835</v>
+      </c>
+    </row>
+    <row r="367" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A367" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B367" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C367" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="D367" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E367" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F367" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="G367" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H367" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I367" s="25"/>
+      <c r="J367" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="K367" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="M367" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="O367" s="2">
+        <v>27025835</v>
+      </c>
     </row>
     <row r="368" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A368" s="28" t="s">
@@ -15361,10 +15376,10 @@
         <v>21</v>
       </c>
       <c r="C368" s="28" t="s">
-        <v>168</v>
+        <v>313</v>
       </c>
       <c r="D368" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E368" s="28" t="s">
         <v>22</v>
@@ -15383,27 +15398,24 @@
         <v>355</v>
       </c>
       <c r="O368" s="2">
-        <v>26822022</v>
+        <v>25614962</v>
       </c>
     </row>
     <row r="369" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A369" s="28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B369" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C369" s="28" t="s">
-        <v>169</v>
+        <v>274</v>
       </c>
       <c r="D369" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E369" s="28" t="s">
         <v>22</v>
-      </c>
-      <c r="F369" s="28" t="s">
-        <v>316</v>
       </c>
       <c r="G369" s="28" t="s">
         <v>115</v>
@@ -15413,36 +15425,30 @@
       </c>
       <c r="I369" s="25"/>
       <c r="J369" s="28" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K369" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="M369" s="28" t="s">
-        <v>314</v>
-      </c>
       <c r="O369" s="2">
-        <v>27025835</v>
+        <v>25614962</v>
       </c>
     </row>
     <row r="370" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A370" s="28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B370" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C370" s="28" t="s">
-        <v>182</v>
+        <v>312</v>
       </c>
       <c r="D370" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E370" s="28" t="s">
         <v>22</v>
-      </c>
-      <c r="F370" s="28" t="s">
-        <v>316</v>
       </c>
       <c r="G370" s="28" t="s">
         <v>115</v>
@@ -15452,27 +15458,24 @@
       </c>
       <c r="I370" s="25"/>
       <c r="J370" s="28" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K370" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="M370" s="28" t="s">
-        <v>314</v>
-      </c>
       <c r="O370" s="2">
-        <v>27025835</v>
+        <v>25614962</v>
       </c>
     </row>
     <row r="371" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A371" s="28" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B371" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C371" s="28" t="s">
-        <v>313</v>
+        <v>181</v>
       </c>
       <c r="D371" s="28" t="s">
         <v>23</v>
@@ -15488,24 +15491,24 @@
       </c>
       <c r="I371" s="25"/>
       <c r="J371" s="28" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="K371" s="18" t="s">
         <v>355</v>
       </c>
       <c r="O371" s="2">
-        <v>25614962</v>
+        <v>29146520</v>
       </c>
     </row>
     <row r="372" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A372" s="28" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B372" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C372" s="28" t="s">
-        <v>274</v>
+        <v>182</v>
       </c>
       <c r="D372" s="28" t="s">
         <v>23</v>
@@ -15521,27 +15524,27 @@
       </c>
       <c r="I372" s="25"/>
       <c r="J372" s="28" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="K372" s="18" t="s">
         <v>355</v>
       </c>
       <c r="O372" s="2">
-        <v>25614962</v>
+        <v>29146520</v>
       </c>
     </row>
     <row r="373" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A373" s="28" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B373" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C373" s="28" t="s">
-        <v>312</v>
+        <v>165</v>
       </c>
       <c r="D373" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E373" s="28" t="s">
         <v>22</v>
@@ -15554,24 +15557,24 @@
       </c>
       <c r="I373" s="25"/>
       <c r="J373" s="28" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="K373" s="18" t="s">
         <v>355</v>
       </c>
       <c r="O373" s="2">
-        <v>25614962</v>
+        <v>29146520</v>
       </c>
     </row>
     <row r="374" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A374" s="28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B374" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C374" s="28" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="D374" s="28" t="s">
         <v>23</v>
@@ -15598,13 +15601,13 @@
     </row>
     <row r="375" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A375" s="28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B375" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C375" s="28" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="D375" s="28" t="s">
         <v>23</v>
@@ -15630,14 +15633,14 @@
       </c>
     </row>
     <row r="376" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A376" s="28" t="s">
+      <c r="A376" s="28">
         <v>4</v>
       </c>
       <c r="B376" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C376" s="28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D376" s="28" t="s">
         <v>23</v>
@@ -15663,14 +15666,14 @@
       </c>
     </row>
     <row r="377" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A377" s="28" t="s">
-        <v>3</v>
+      <c r="A377" s="28">
+        <v>4</v>
       </c>
       <c r="B377" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C377" s="28" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="D377" s="28" t="s">
         <v>23</v>
@@ -15696,8 +15699,8 @@
       </c>
     </row>
     <row r="378" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A378" s="28" t="s">
-        <v>3</v>
+      <c r="A378" s="28">
+        <v>4</v>
       </c>
       <c r="B378" s="28" t="s">
         <v>21</v>
@@ -15729,20 +15732,20 @@
       </c>
     </row>
     <row r="379" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A379" s="28">
-        <v>4</v>
+      <c r="A379" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="B379" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C379" s="28" t="s">
-        <v>161</v>
+        <v>276</v>
       </c>
       <c r="D379" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E379" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G379" s="28" t="s">
         <v>115</v>
@@ -15752,24 +15755,24 @@
       </c>
       <c r="I379" s="25"/>
       <c r="J379" s="28" t="s">
-        <v>345</v>
-      </c>
-      <c r="K379" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="K379" s="36" t="s">
         <v>355</v>
       </c>
       <c r="O379" s="2">
-        <v>29146520</v>
+        <v>30125371</v>
       </c>
     </row>
     <row r="380" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A380" s="28">
-        <v>4</v>
+      <c r="A380" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="B380" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C380" s="28" t="s">
-        <v>183</v>
+        <v>317</v>
       </c>
       <c r="D380" s="28" t="s">
         <v>23</v>
@@ -15785,24 +15788,24 @@
       </c>
       <c r="I380" s="25"/>
       <c r="J380" s="28" t="s">
-        <v>345</v>
-      </c>
-      <c r="K380" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="K380" s="36" t="s">
         <v>355</v>
       </c>
       <c r="O380" s="2">
-        <v>29146520</v>
+        <v>30125371</v>
       </c>
     </row>
     <row r="381" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A381" s="28">
-        <v>4</v>
+      <c r="A381" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="B381" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C381" s="28" t="s">
-        <v>168</v>
+        <v>318</v>
       </c>
       <c r="D381" s="28" t="s">
         <v>23</v>
@@ -15818,24 +15821,24 @@
       </c>
       <c r="I381" s="25"/>
       <c r="J381" s="28" t="s">
-        <v>345</v>
-      </c>
-      <c r="K381" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="K381" s="36" t="s">
         <v>355</v>
       </c>
       <c r="O381" s="2">
-        <v>29146520</v>
+        <v>30125371</v>
       </c>
     </row>
     <row r="382" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A382" s="28" t="s">
-        <v>139</v>
+        <v>319</v>
       </c>
       <c r="B382" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C382" s="28" t="s">
-        <v>276</v>
+        <v>320</v>
       </c>
       <c r="D382" s="28" t="s">
         <v>22</v>
@@ -15851,207 +15854,108 @@
       </c>
       <c r="I382" s="25"/>
       <c r="J382" s="28" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="K382" s="36" t="s">
         <v>355</v>
       </c>
       <c r="O382" s="2">
-        <v>30125371</v>
+        <v>28789880</v>
       </c>
     </row>
     <row r="383" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A383" s="28" t="s">
-        <v>139</v>
+        <v>6</v>
       </c>
       <c r="B383" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C383" s="28" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="D383" s="28" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E383" s="28" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="F383" s="28" t="s">
+        <v>2</v>
       </c>
       <c r="G383" s="28" t="s">
         <v>115</v>
       </c>
       <c r="H383" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="I383" s="25"/>
-      <c r="J383" s="28" t="s">
-        <v>344</v>
-      </c>
-      <c r="K383" s="36" t="s">
-        <v>355</v>
+        <v>5</v>
+      </c>
+      <c r="I383" s="25" t="s">
+        <v>348</v>
       </c>
       <c r="O383" s="2">
-        <v>30125371</v>
+        <v>29425396</v>
       </c>
     </row>
     <row r="384" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A384" s="28" t="s">
-        <v>139</v>
+        <v>6</v>
       </c>
       <c r="B384" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C384" s="28" t="s">
-        <v>318</v>
+        <v>215</v>
       </c>
       <c r="D384" s="28" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E384" s="28" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="F384" s="28" t="s">
+        <v>2</v>
       </c>
       <c r="G384" s="28" t="s">
         <v>115</v>
       </c>
       <c r="H384" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="I384" s="25"/>
-      <c r="J384" s="28" t="s">
-        <v>344</v>
-      </c>
-      <c r="K384" s="36" t="s">
-        <v>355</v>
+        <v>5</v>
+      </c>
+      <c r="I384" s="25" t="s">
+        <v>348</v>
       </c>
       <c r="O384" s="2">
-        <v>30125371</v>
+        <v>29425396</v>
       </c>
     </row>
     <row r="385" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385" s="28" t="s">
-        <v>319</v>
+        <v>6</v>
       </c>
       <c r="B385" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C385" s="28" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
       <c r="D385" s="28" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E385" s="28" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="F385" s="28" t="s">
+        <v>2</v>
       </c>
       <c r="G385" s="28" t="s">
         <v>115</v>
       </c>
       <c r="H385" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="I385" s="25"/>
-      <c r="J385" s="28" t="s">
-        <v>321</v>
-      </c>
-      <c r="K385" s="36" t="s">
-        <v>355</v>
+        <v>5</v>
+      </c>
+      <c r="I385" s="25" t="s">
+        <v>348</v>
       </c>
       <c r="O385" s="2">
-        <v>28789880</v>
-      </c>
-    </row>
-    <row r="386" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A386" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B386" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C386" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="D386" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E386" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="F386" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="G386" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H386" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="I386" s="25" t="s">
-        <v>348</v>
-      </c>
-      <c r="O386" s="2">
-        <v>29425396</v>
-      </c>
-    </row>
-    <row r="387" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A387" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B387" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C387" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="D387" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E387" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="F387" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="G387" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H387" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="I387" s="25" t="s">
-        <v>348</v>
-      </c>
-      <c r="O387" s="2">
-        <v>29425396</v>
-      </c>
-    </row>
-    <row r="388" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A388" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B388" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C388" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="D388" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E388" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="F388" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="G388" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H388" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="I388" s="25" t="s">
-        <v>348</v>
-      </c>
-      <c r="O388" s="2">
         <v>29425396</v>
       </c>
     </row>

</xml_diff>